<commit_message>
udpated excelsheet for formula update
</commit_message>
<xml_diff>
--- a/src/test/resources/financial_data_formula.xlsx
+++ b/src/test/resources/financial_data_formula.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>fitchFieldId</t>
   </si>
@@ -193,12 +193,6 @@
   </si>
   <si>
     <t>FC_NET_INT_INC_BNK/FC_AVG_EARNING_ASSETS_BNK</t>
-  </si>
-  <si>
-    <t>FC_NON_INT_EXP_GROSS_REV_BNK</t>
-  </si>
-  <si>
-    <t>FC_TOTAL_NON_INT_EXP_BNK/(FC_GROSS_INT_DIV_INC_BNK+FC_NET_INT_INC_BNK)</t>
   </si>
   <si>
     <t>FC_TANGIBLE_COMMON_EQUITY_TANGIBLE_ASSETS_BNK</t>
@@ -655,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -712,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -720,7 +714,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -776,7 +770,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -947,7 +941,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -969,19 +963,6 @@
       </c>
       <c r="B38" s="2" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -991,17 +972,17 @@
     </cfRule>
     <cfRule type="duplicateValues" dxfId="4" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
+  <conditionalFormatting sqref="B37">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>IF(FIND(" ",$A38)&gt;0,TRUE,FALSE)</formula>
+      <formula>IF(FIND(" ",$A37)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A39">
-    <cfRule type="expression" dxfId="1" priority="11">
+  <conditionalFormatting sqref="A2:A38">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>IF(FIND(" ",$A2)&gt;0,TRUE,FALSE)</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="14"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>